<commit_message>
Update job calc for haswell
</commit_message>
<xml_diff>
--- a/VSC/Credit_calcul.xlsx
+++ b/VSC/Credit_calcul.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>(0,000278*WALLTIME*NODES + 0,1) * NODETYPE</t>
   </si>
@@ -334,7 +334,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -342,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G10"/>
+  <dimension ref="B4:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -400,6 +400,51 @@
         <v>51.127802160791589</v>
       </c>
     </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>B14/6.68</f>
+        <v>299.40119760479041</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>B15-0.1</f>
+        <v>299.30119760479039</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>B16/0.000278</f>
+        <v>1076623.012966872</v>
+      </c>
+      <c r="C17">
+        <f>B17/60</f>
+        <v>17943.716882781198</v>
+      </c>
+      <c r="D17">
+        <f>C17/60</f>
+        <v>299.06194804635328</v>
+      </c>
+      <c r="E17">
+        <f>D17/24</f>
+        <v>12.460914501931386</v>
+      </c>
+      <c r="G17">
+        <f>(D17-299) * 60</f>
+        <v>3.7168827811967731</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>